<commit_message>
Adding stemmed text and alignments
</commit_message>
<xml_diff>
--- a/hw1/Results/EM Model2.xlsx
+++ b/hw1/Results/EM Model2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>number</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>No diag growth</t>
+  </si>
+  <si>
+    <t>Stemmed</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -497,7 +500,12 @@
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:7">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -516,8 +524,11 @@
       <c r="F2" s="1">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -536,8 +547,11 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -556,8 +570,11 @@
       <c r="F4">
         <v>0.394673</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.36879400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -576,8 +593,11 @@
       <c r="F5">
         <v>0.58196700000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0.59055100000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -596,8 +616,11 @@
       <c r="F6">
         <v>0.63905299999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>0.69230800000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -616,8 +639,11 @@
       <c r="F7">
         <v>0.27114700000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>0.28571400000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -636,8 +662,11 @@
       <c r="F8">
         <v>0.67047599999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>0.68143500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -656,8 +685,11 @@
       <c r="F9">
         <v>0.81952700000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0.760355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -676,8 +708,11 @@
       <c r="F10">
         <v>0.31323000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>0.30713499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -696,8 +731,11 @@
       <c r="F11">
         <v>0.59710099999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>0.61049299999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -716,8 +754,11 @@
       <c r="F12">
         <v>0.86982199999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>0.84615399999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -736,8 +777,11 @@
       <c r="F13">
         <v>0.36006100000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>0.35745300000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -756,8 +800,11 @@
       <c r="F14">
         <v>0.69349799999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>0.67705400000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -776,8 +823,11 @@
       <c r="F15">
         <v>0.58875699999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>0.60650899999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -787,8 +837,11 @@
       <c r="F16">
         <v>0.38197999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>0.35452299999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -798,8 +851,11 @@
       <c r="F17">
         <v>0.60666699999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>0.61458299999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -809,23 +865,26 @@
       <c r="F18">
         <v>0.63313600000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G18">
+        <v>0.68934899999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="F23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="F24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="F25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="F26" t="s">
         <v>24</v>
       </c>

</xml_diff>